<commit_message>
Deploying to gh-pages from @ IDGRLP/Tumorkonferenzen-IG@c2716517def48a1cd47c75767621b1a7e68409b7 🚀
</commit_message>
<xml_diff>
--- a/site/CodeSystem-HistoGrade.xlsx
+++ b/site/CodeSystem-HistoGrade.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://krebsregister-rlp.de/fhir/tumorboard/CodeSystem/HistoGrade</t>
+    <t>http://idg-rlp.de/fhir/tumorkonferenzen/CodeSystem/HistoGrade</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-29T10:35:30+00:00</t>
+    <t>2024-04-07T13:52:57+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>